<commit_message>
feat(import): include product note in import feature
</commit_message>
<xml_diff>
--- a/public/assets/product-import-example.xlsx
+++ b/public/assets/product-import-example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndreasVifert\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\anvi\dev\nem-lager\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD2624D1-1C73-462B-8EB0-6EF9AC061D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438E6AF2-ACC0-4A48-9EF3-D4CC7F99EE24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2D44D5FF-43E7-43AC-89ED-A146F6506CAF}"/>
+    <workbookView xWindow="30225" yWindow="1425" windowWidth="21600" windowHeight="11295" xr2:uid="{2D44D5FF-43E7-43AC-89ED-A146F6506CAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>sku</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>nej</t>
+  </si>
+  <si>
+    <t>note</t>
   </si>
 </sst>
 </file>
@@ -455,15 +458,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A43A86C6-31E3-4BF8-AAE3-8B62D49F77B5}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -492,10 +495,13 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -520,7 +526,7 @@
       <c r="I2">
         <v>14.4</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(import): new product import example
</commit_message>
<xml_diff>
--- a/public/assets/product-import-example.xlsx
+++ b/public/assets/product-import-example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\anvi\dev\nem-lager\public\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TobiasHorneChristian\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438E6AF2-ACC0-4A48-9EF3-D4CC7F99EE24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E126D38D-57C9-47E5-9E4F-556580F4BFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30225" yWindow="1425" windowWidth="21600" windowHeight="11295" xr2:uid="{2D44D5FF-43E7-43AC-89ED-A146F6506CAF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2D44D5FF-43E7-43AC-89ED-A146F6506CAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>sku</t>
   </si>
@@ -87,16 +87,61 @@
   </si>
   <si>
     <t>note</t>
+  </si>
+  <si>
+    <t>V00002</t>
+  </si>
+  <si>
+    <t>Gruppe2</t>
+  </si>
+  <si>
+    <t>Vare 2</t>
+  </si>
+  <si>
+    <t>minimum</t>
+  </si>
+  <si>
+    <t>maximum</t>
+  </si>
+  <si>
+    <t>orderAmount</t>
+  </si>
+  <si>
+    <t>V00003</t>
+  </si>
+  <si>
+    <t>Gruppe3</t>
+  </si>
+  <si>
+    <t>Vare 3</t>
+  </si>
+  <si>
+    <t>Liter</t>
+  </si>
+  <si>
+    <t>Diverse</t>
+  </si>
+  <si>
+    <t>V00004</t>
+  </si>
+  <si>
+    <t>Vare 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -122,8 +167,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,15 +505,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A43A86C6-31E3-4BF8-AAE3-8B62D49F77B5}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -500,8 +547,17 @@
       <c r="K1" t="s">
         <v>9</v>
       </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -529,8 +585,120 @@
       <c r="K2" t="s">
         <v>15</v>
       </c>
+      <c r="L2">
+        <v>35</v>
+      </c>
+      <c r="M2">
+        <v>50</v>
+      </c>
+      <c r="N2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3">
+        <v>10.6</v>
+      </c>
+      <c r="I3">
+        <v>14.4</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4">
+        <v>10.6</v>
+      </c>
+      <c r="I4">
+        <v>14.4</v>
+      </c>
+      <c r="K4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4">
+        <v>25</v>
+      </c>
+      <c r="N4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5">
+        <v>10.6</v>
+      </c>
+      <c r="I5">
+        <v>14.4</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="1">
+        <v>2500.5</v>
+      </c>
+      <c r="M5" s="2">
+        <v>5000</v>
+      </c>
+      <c r="N5">
+        <v>3000</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>